<commit_message>
Created the initial parameters for membership list expectations. All but 1 test pass
</commit_message>
<xml_diff>
--- a/tests/fakeodsa.xlsx
+++ b/tests/fakeodsa.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="63">
   <si>
     <t xml:space="preserve">AK_ID</t>
   </si>
@@ -151,33 +151,36 @@
     <t xml:space="preserve">annual</t>
   </si>
   <si>
+    <t xml:space="preserve">active</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Elsesson</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4444 Fake Way</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Winter Park</t>
+  </si>
+  <si>
+    <t xml:space="preserve">32789-1955</t>
+  </si>
+  <si>
+    <t xml:space="preserve">burp@derp.nl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3/29/2017</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11/1/2099</t>
+  </si>
+  <si>
     <t xml:space="preserve">never</t>
   </si>
   <si>
-    <t xml:space="preserve">Elsesson</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4444 Fake Way</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Winter Park</t>
-  </si>
-  <si>
-    <t xml:space="preserve">32789-1955</t>
-  </si>
-  <si>
-    <t xml:space="preserve">burp@derp.nl</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3/29/2017</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11/1/2099</t>
-  </si>
-  <si>
     <t xml:space="preserve">Megan</t>
   </si>
   <si>
@@ -203,6 +206,9 @@
   </si>
   <si>
     <t xml:space="preserve">2mo_plus_failed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">canceled_by_admin</t>
   </si>
 </sst>
 </file>
@@ -214,11 +220,12 @@
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -240,11 +247,6 @@
       <name val="Times New Roman"/>
       <family val="1"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -289,7 +291,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -306,16 +308,8 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -335,10 +329,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Z4"/>
+  <dimension ref="A1:Z5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="R11" activeCellId="0" sqref="R11"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -428,7 +422,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="n">
         <v>12345</v>
       </c>
@@ -518,7 +512,7 @@
       <c r="M3" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="N3" s="4" t="s">
+      <c r="N3" s="2" t="s">
         <v>48</v>
       </c>
       <c r="O3" s="1" t="s">
@@ -533,13 +527,14 @@
       <c r="T3" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="U3" s="5" t="b">
+      <c r="U3" s="4" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="V3" s="6" t="s">
+      <c r="V3" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="W3" s="6" t="s">
+      <c r="W3" s="3" t="s">
         <v>51</v>
       </c>
       <c r="X3" s="1" t="s">
@@ -549,60 +544,65 @@
         <v>42</v>
       </c>
       <c r="Z3" s="1" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4" t="n">
+      <c r="A4" s="2" t="n">
         <v>4845</v>
       </c>
-      <c r="B4" s="4" t="n">
+      <c r="B4" s="2" t="n">
         <v>222897</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="L4" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="M4" s="4" t="s">
+      <c r="L4" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="M4" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="N4" s="4" t="s">
-        <v>55</v>
+      <c r="N4" s="2" t="s">
+        <v>56</v>
       </c>
       <c r="O4" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="Q4" s="4" t="n">
+      <c r="Q4" s="2" t="n">
         <v>4077217359</v>
       </c>
       <c r="S4" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="T4" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="T4" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="U4" s="6" t="s">
+      <c r="U4" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="V4" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="W4" s="6" t="s">
+      <c r="V4" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="X4" s="4" t="s">
+      <c r="W4" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="X4" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="Y4" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="Z4" s="4" t="s">
+      <c r="Y4" s="2" t="s">
         <v>60</v>
+      </c>
+      <c r="Z4" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="Z5" s="1" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Final verification test fails due to a condition of the spreadsheet used and to errors with phone numbers, city, and state
</commit_message>
<xml_diff>
--- a/tests/fakeodsa.xlsx
+++ b/tests/fakeodsa.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="62">
   <si>
     <t xml:space="preserve">AK_ID</t>
   </si>
@@ -206,9 +206,6 @@
   </si>
   <si>
     <t xml:space="preserve">2mo_plus_failed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">canceled_by_admin</t>
   </si>
 </sst>
 </file>
@@ -329,10 +326,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Z5"/>
+  <dimension ref="A1:Z4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="Z5" activeCellId="0" sqref="Z5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -600,11 +597,6 @@
         <v>61</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z5" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Failing test to return False on a list with only soft errors
</commit_message>
<xml_diff>
--- a/tests/fakeodsa.xlsx
+++ b/tests/fakeodsa.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="65">
   <si>
     <t xml:space="preserve">AK_ID</t>
   </si>
@@ -127,7 +127,7 @@
     <t xml:space="preserve">United States</t>
   </si>
   <si>
-    <t xml:space="preserve">410-5644639, 4105644639</t>
+    <t xml:space="preserve">410-564-4639</t>
   </si>
   <si>
     <t xml:space="preserve">mattprime@gmail.com</t>
@@ -169,6 +169,9 @@
     <t xml:space="preserve">32789-1955</t>
   </si>
   <si>
+    <t xml:space="preserve">407-444-0909</t>
+  </si>
+  <si>
     <t xml:space="preserve">burp@derp.nl</t>
   </si>
   <si>
@@ -184,6 +187,9 @@
     <t xml:space="preserve">Megan</t>
   </si>
   <si>
+    <t xml:space="preserve">Dumbface</t>
+  </si>
+  <si>
     <t xml:space="preserve">87 Nope Ln</t>
   </si>
   <si>
@@ -191,6 +197,9 @@
   </si>
   <si>
     <t xml:space="preserve">32779-3004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">407-721-7359</t>
   </si>
   <si>
     <t xml:space="preserve">fsa@gmail.com</t>
@@ -329,7 +338,7 @@
   <dimension ref="A1:Z4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Z5" activeCellId="0" sqref="Z5"/>
+      <selection pane="topLeft" activeCell="Q4" activeCellId="0" sqref="Q4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -515,11 +524,11 @@
       <c r="O3" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="P3" s="1" t="n">
-        <v>4074440909</v>
+      <c r="P3" s="1" t="s">
+        <v>49</v>
       </c>
       <c r="S3" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="T3" s="1" t="s">
         <v>37</v>
@@ -529,10 +538,10 @@
         <v>0</v>
       </c>
       <c r="V3" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="W3" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="X3" s="1" t="s">
         <v>41</v>
@@ -541,10 +550,10 @@
         <v>42</v>
       </c>
       <c r="Z3" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="n">
         <v>4845</v>
       </c>
@@ -552,28 +561,31 @@
         <v>222897</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>55</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="M4" s="2" t="s">
         <v>32</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="O4" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="Q4" s="2" t="n">
-        <v>4077217359</v>
+      <c r="Q4" s="2" t="s">
+        <v>59</v>
       </c>
       <c r="S4" s="1" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="T4" s="2" t="s">
         <v>37</v>
@@ -582,19 +594,19 @@
         <v>38</v>
       </c>
       <c r="V4" s="3" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="W4" s="3" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="X4" s="2" t="s">
         <v>41</v>
       </c>
       <c r="Y4" s="2" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="Z4" s="2" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Refactored verify_memlist_data_integrity to return False when only soft failures are encountered
</commit_message>
<xml_diff>
--- a/tests/fakeodsa.xlsx
+++ b/tests/fakeodsa.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="66">
   <si>
     <t xml:space="preserve">AK_ID</t>
   </si>
@@ -161,6 +161,9 @@
   </si>
   <si>
     <t xml:space="preserve">4444 Fake Way</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Appartment 4</t>
   </si>
   <si>
     <t xml:space="preserve">Winter Park</t>
@@ -338,7 +341,7 @@
   <dimension ref="A1:Z4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q4" activeCellId="0" sqref="Q4"/>
+      <selection pane="topLeft" activeCell="K3" activeCellId="0" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -509,26 +512,26 @@
       <c r="J3" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="K3" s="1" t="n">
-        <v>4</v>
+      <c r="K3" s="1" t="s">
+        <v>47</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="M3" s="1" t="s">
         <v>32</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="O3" s="1" t="s">
         <v>34</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="S3" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="T3" s="1" t="s">
         <v>37</v>
@@ -538,10 +541,10 @@
         <v>0</v>
       </c>
       <c r="V3" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="W3" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="X3" s="1" t="s">
         <v>41</v>
@@ -550,7 +553,7 @@
         <v>42</v>
       </c>
       <c r="Z3" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -561,31 +564,31 @@
         <v>222897</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="M4" s="2" t="s">
         <v>32</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="O4" s="1" t="s">
         <v>34</v>
       </c>
       <c r="Q4" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="S4" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="T4" s="2" t="s">
         <v>37</v>
@@ -594,19 +597,19 @@
         <v>38</v>
       </c>
       <c r="V4" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="W4" s="3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="X4" s="2" t="s">
         <v>41</v>
       </c>
       <c r="Y4" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="Z4" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added a lessthanideal list to show all 3 possible acceptable outcomes to verify_memlist_integrity
</commit_message>
<xml_diff>
--- a/tests/fakeodsa.xlsx
+++ b/tests/fakeodsa.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="62">
   <si>
     <t xml:space="preserve">AK_ID</t>
   </si>
@@ -127,7 +127,7 @@
     <t xml:space="preserve">United States</t>
   </si>
   <si>
-    <t xml:space="preserve">410-564-4639</t>
+    <t xml:space="preserve">410-5644639, 4105644639</t>
   </si>
   <si>
     <t xml:space="preserve">mattprime@gmail.com</t>
@@ -163,18 +163,12 @@
     <t xml:space="preserve">4444 Fake Way</t>
   </si>
   <si>
-    <t xml:space="preserve">Appartment 4</t>
-  </si>
-  <si>
     <t xml:space="preserve">Winter Park</t>
   </si>
   <si>
     <t xml:space="preserve">32789-1955</t>
   </si>
   <si>
-    <t xml:space="preserve">407-444-0909</t>
-  </si>
-  <si>
     <t xml:space="preserve">burp@derp.nl</t>
   </si>
   <si>
@@ -190,9 +184,6 @@
     <t xml:space="preserve">Megan</t>
   </si>
   <si>
-    <t xml:space="preserve">Dumbface</t>
-  </si>
-  <si>
     <t xml:space="preserve">87 Nope Ln</t>
   </si>
   <si>
@@ -200,9 +191,6 @@
   </si>
   <si>
     <t xml:space="preserve">32779-3004</t>
-  </si>
-  <si>
-    <t xml:space="preserve">407-721-7359</t>
   </si>
   <si>
     <t xml:space="preserve">fsa@gmail.com</t>
@@ -341,7 +329,7 @@
   <dimension ref="A1:Z4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K3" activeCellId="0" sqref="K3"/>
+      <selection pane="topLeft" activeCell="Z5" activeCellId="0" sqref="Z5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -512,26 +500,26 @@
       <c r="J3" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="K3" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="L3" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>48</v>
       </c>
       <c r="M3" s="1" t="s">
         <v>32</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="O3" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="P3" s="1" t="s">
-        <v>50</v>
+      <c r="P3" s="1" t="n">
+        <v>4074440909</v>
       </c>
       <c r="S3" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="T3" s="1" t="s">
         <v>37</v>
@@ -541,10 +529,10 @@
         <v>0</v>
       </c>
       <c r="V3" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="W3" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="X3" s="1" t="s">
         <v>41</v>
@@ -553,10 +541,10 @@
         <v>42</v>
       </c>
       <c r="Z3" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="n">
         <v>4845</v>
       </c>
@@ -564,31 +552,28 @@
         <v>222897</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="L4" s="2" t="s">
         <v>55</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="L4" s="2" t="s">
-        <v>58</v>
       </c>
       <c r="M4" s="2" t="s">
         <v>32</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="O4" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="Q4" s="2" t="s">
-        <v>60</v>
+      <c r="Q4" s="2" t="n">
+        <v>4077217359</v>
       </c>
       <c r="S4" s="1" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="T4" s="2" t="s">
         <v>37</v>
@@ -597,19 +582,19 @@
         <v>38</v>
       </c>
       <c r="V4" s="3" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="W4" s="3" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="X4" s="2" t="s">
         <v>41</v>
       </c>
       <c r="Y4" s="2" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="Z4" s="2" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
RED on get failure refactor
</commit_message>
<xml_diff>
--- a/tests/fakeodsa.xlsx
+++ b/tests/fakeodsa.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="63">
   <si>
     <t xml:space="preserve">AK_ID</t>
   </si>
@@ -161,6 +161,9 @@
   </si>
   <si>
     <t xml:space="preserve">4444 Fake Way</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bldg 4</t>
   </si>
   <si>
     <t xml:space="preserve">Winter Park</t>
@@ -329,7 +332,7 @@
   <dimension ref="A1:Z4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Z5" activeCellId="0" sqref="Z5"/>
+      <selection pane="topLeft" activeCell="K3" activeCellId="0" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -500,17 +503,17 @@
       <c r="J3" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="K3" s="1" t="n">
-        <v>4</v>
+      <c r="K3" s="1" t="s">
+        <v>47</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="M3" s="1" t="s">
         <v>32</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="O3" s="1" t="s">
         <v>34</v>
@@ -519,7 +522,7 @@
         <v>4074440909</v>
       </c>
       <c r="S3" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="T3" s="1" t="s">
         <v>37</v>
@@ -529,10 +532,10 @@
         <v>0</v>
       </c>
       <c r="V3" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="W3" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="X3" s="1" t="s">
         <v>41</v>
@@ -541,7 +544,7 @@
         <v>42</v>
       </c>
       <c r="Z3" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -552,19 +555,19 @@
         <v>222897</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="M4" s="2" t="s">
         <v>32</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="O4" s="1" t="s">
         <v>34</v>
@@ -573,7 +576,7 @@
         <v>4077217359</v>
       </c>
       <c r="S4" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="T4" s="2" t="s">
         <v>37</v>
@@ -582,19 +585,19 @@
         <v>38</v>
       </c>
       <c r="V4" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="W4" s="3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="X4" s="2" t="s">
         <v>41</v>
       </c>
       <c r="Y4" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="Z4" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>